<commit_message>
drivers with no other expanded
</commit_message>
<xml_diff>
--- a/data/refined_drivers/otherclimatedrivers_lookup.xlsx
+++ b/data/refined_drivers/otherclimatedrivers_lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annalopresti/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\Documents\GitHub\BCCAch7\data\refined_drivers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{375ABBDB-2172-CD4B-A68F-09F2D9E2886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0361A0B9-F298-4CF5-BFEF-560D60592673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="520" windowWidth="14380" windowHeight="16440" activeTab="1" xr2:uid="{2621AD7F-AB1A-E74A-BB38-AD63999953F2}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{2621AD7F-AB1A-E74A-BB38-AD63999953F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>raw</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>need to know what kind of ice in order to code this</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>surface water change</t>
@@ -614,17 +611,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8994F6-F41D-6944-BEB6-66E836A5D57A}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="60.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="60.1484375" customWidth="1"/>
+    <col min="2" max="2" width="21.1484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +632,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -643,7 +640,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -654,7 +651,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -662,7 +659,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -673,7 +670,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -681,7 +678,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -689,7 +686,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -697,7 +694,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -705,7 +702,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -713,7 +710,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -721,7 +718,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -729,34 +726,34 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -764,7 +761,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -772,7 +769,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -780,7 +777,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -788,7 +785,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -796,18 +793,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
         <v>54</v>
       </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -815,7 +812,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -823,23 +820,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -847,15 +844,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -863,7 +860,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -871,15 +868,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -887,7 +884,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -895,23 +892,23 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -919,15 +916,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -944,94 +941,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F89E10-CA8D-FC46-9106-B1361C4EBA63}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A7" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A12" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>